<commit_message>
add 8 more test cases for Trulia MortgagePage and add a helper method at Base Class
</commit_message>
<xml_diff>
--- a/com.trulia/src/test/resources/Trulia.xlsx
+++ b/com.trulia/src/test/resources/Trulia.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdaziz/IdeaProjects/Team1BootCamp/com.trulia/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60E1BDF-8DBF-2843-AD2F-4E1CB34DD582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E01DEB-6A17-3548-A722-484986896604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="DropDownList" sheetId="1" r:id="rId1"/>
-    <sheet name="Ebay" sheetId="2" r:id="rId2"/>
+    <sheet name="MortgageCalculator" sheetId="2" r:id="rId2"/>
     <sheet name="CBSSports" sheetId="3" r:id="rId3"/>
     <sheet name="ATT" sheetId="4" r:id="rId4"/>
     <sheet name="BankOfAmerica" sheetId="5" r:id="rId5"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>A</t>
   </si>
@@ -74,13 +74,97 @@
   </si>
   <si>
     <t>Refinance Calculator</t>
+  </si>
+  <si>
+    <t>purchase price</t>
+  </si>
+  <si>
+    <t>down payment%</t>
+  </si>
+  <si>
+    <t>300000</t>
+  </si>
+  <si>
+    <t>Loan Type</t>
+  </si>
+  <si>
+    <t>30-Year Fixed</t>
+  </si>
+  <si>
+    <t>20-Year Fixed</t>
+  </si>
+  <si>
+    <t>15-Year Fixed</t>
+  </si>
+  <si>
+    <t>10-Year Fixed</t>
+  </si>
+  <si>
+    <t>FHA 30-Year Fixed</t>
+  </si>
+  <si>
+    <t>FHA 15-Year Fixed</t>
+  </si>
+  <si>
+    <t>VA 30-Year Fixed</t>
+  </si>
+  <si>
+    <t>VA 15-Year Fixed</t>
+  </si>
+  <si>
+    <t>Expected Mortgage Payment</t>
+  </si>
+  <si>
+    <t>400000</t>
+  </si>
+  <si>
+    <t>250000</t>
+  </si>
+  <si>
+    <t>325000</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>$1,490</t>
+  </si>
+  <si>
+    <t>$3,238</t>
+  </si>
+  <si>
+    <t>$915</t>
+  </si>
+  <si>
+    <t>$1,565</t>
+  </si>
+  <si>
+    <t>$1,266</t>
+  </si>
+  <si>
+    <t>$2,015</t>
+  </si>
+  <si>
+    <t>$1,551</t>
+  </si>
+  <si>
+    <t>$2,742</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +177,13 @@
       <color rgb="FF202124"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,9 +206,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16D271-5906-41EE-853E-85EA245B6942}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -485,6 +579,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -560,14 +655,147 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751B09C-FE73-4F13-A91B-81E55B55AAEA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>